<commit_message>
Begindocumenten (nieuwste versie) + groepsverslag
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26216"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="235" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54A631A4-FD86-4405-BF03-C1EEE51BDFC6}"/>
+  <xr:revisionPtr revIDLastSave="336" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A9A2EF2-A254-4A3B-A6E2-54D9E78014D5}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>Week 1</t>
   </si>
@@ -99,16 +99,55 @@
     <t>W</t>
   </si>
   <si>
-    <t>1.1 - 1.6</t>
-  </si>
-  <si>
-    <t>1.7 - 1.9</t>
-  </si>
-  <si>
-    <t>3.1 - 3.4</t>
-  </si>
-  <si>
-    <t>3.5 - 3.9</t>
+    <t>1.1 - 1.6: Opdracht Verkennen en Structuur  Creeren</t>
+  </si>
+  <si>
+    <t>1.7 - 1.9: Materiaalselectie en Kostenraming</t>
+  </si>
+  <si>
+    <t>2.1: Afzonderlijke 3D modellen</t>
+  </si>
+  <si>
+    <t>2.2: Assemblage 3D-onderdelen</t>
+  </si>
+  <si>
+    <t>2.3: Technisch Tekenen</t>
+  </si>
+  <si>
+    <t>2.4: Stuklijst</t>
+  </si>
+  <si>
+    <t>3.1 - 3.2: Coderen MIcrocontroller en Besturing</t>
+  </si>
+  <si>
+    <t>3.3: Testen Afzonderlijke Onderdelen en Mogelijke Aanpassingen</t>
+  </si>
+  <si>
+    <t>3.4: Alles in Elkaar Steken</t>
+  </si>
+  <si>
+    <t>3.5: Geheel Testen</t>
+  </si>
+  <si>
+    <t>3.6: Aanpassingen maken</t>
+  </si>
+  <si>
+    <t>4.2 - 4.3: Inleiding en Probleem Schetsen</t>
+  </si>
+  <si>
+    <t>4.4: Ontwerpproces en Materiaalselectie Illustreren</t>
+  </si>
+  <si>
+    <t>4.5 - 4.6: Elektronisch Circuit en Programmeren</t>
+  </si>
+  <si>
+    <t>4.7 &amp; 4.9: Resultaten, Mogelijke Verbeteringen en Besluit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>4.8: Financieel Rapport</t>
   </si>
 </sst>
 </file>
@@ -165,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,23 +215,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,257 +548,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CX20"/>
+  <dimension ref="A1:CX41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A20"/>
+    <sheetView tabSelected="1" topLeftCell="CD7" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="57.5703125" style="9" customWidth="1"/>
     <col min="2" max="100" width="3.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:102">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4" t="s">
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4" t="s">
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="4"/>
-      <c r="AN1" s="4" t="s">
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AO1" s="4"/>
-      <c r="AP1" s="4"/>
-      <c r="AQ1" s="4"/>
-      <c r="AR1" s="4"/>
-      <c r="AS1" s="4"/>
-      <c r="AT1" s="4"/>
-      <c r="AU1" s="4" t="s">
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AV1" s="4"/>
-      <c r="AW1" s="4"/>
-      <c r="AX1" s="4"/>
-      <c r="AY1" s="4"/>
-      <c r="AZ1" s="4"/>
-      <c r="BA1" s="4"/>
-      <c r="BB1" s="4" t="s">
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="4"/>
-      <c r="BD1" s="4"/>
-      <c r="BE1" s="4"/>
-      <c r="BF1" s="4"/>
-      <c r="BG1" s="4"/>
-      <c r="BH1" s="4"/>
-      <c r="BI1" s="4" t="s">
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BJ1" s="4"/>
-      <c r="BK1" s="4"/>
-      <c r="BL1" s="4"/>
-      <c r="BM1" s="4"/>
-      <c r="BN1" s="4"/>
-      <c r="BO1" s="4"/>
-      <c r="BP1" s="4" t="s">
+      <c r="BJ1" s="5"/>
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+      <c r="BM1" s="5"/>
+      <c r="BN1" s="5"/>
+      <c r="BO1" s="5"/>
+      <c r="BP1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="4"/>
-      <c r="BR1" s="4"/>
-      <c r="BS1" s="4"/>
-      <c r="BT1" s="4"/>
-      <c r="BU1" s="4"/>
-      <c r="BV1" s="4"/>
-      <c r="BW1" s="4" t="s">
+      <c r="BQ1" s="5"/>
+      <c r="BR1" s="5"/>
+      <c r="BS1" s="5"/>
+      <c r="BT1" s="5"/>
+      <c r="BU1" s="5"/>
+      <c r="BV1" s="5"/>
+      <c r="BW1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="BX1" s="4"/>
-      <c r="BY1" s="4"/>
-      <c r="BZ1" s="4"/>
-      <c r="CA1" s="4"/>
-      <c r="CB1" s="4"/>
-      <c r="CC1" s="4"/>
-      <c r="CD1" s="4" t="s">
+      <c r="BX1" s="5"/>
+      <c r="BY1" s="5"/>
+      <c r="BZ1" s="5"/>
+      <c r="CA1" s="5"/>
+      <c r="CB1" s="5"/>
+      <c r="CC1" s="5"/>
+      <c r="CD1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="4"/>
-      <c r="CF1" s="4"/>
-      <c r="CG1" s="4"/>
-      <c r="CH1" s="4"/>
-      <c r="CI1" s="4"/>
-      <c r="CJ1" s="4"/>
-      <c r="CK1" s="4" t="s">
+      <c r="CE1" s="5"/>
+      <c r="CF1" s="5"/>
+      <c r="CG1" s="5"/>
+      <c r="CH1" s="5"/>
+      <c r="CI1" s="5"/>
+      <c r="CJ1" s="5"/>
+      <c r="CK1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="CL1" s="4"/>
-      <c r="CM1" s="4"/>
-      <c r="CN1" s="4"/>
-      <c r="CO1" s="4"/>
-      <c r="CP1" s="4"/>
-      <c r="CQ1" s="4"/>
-      <c r="CR1" s="4" t="s">
+      <c r="CL1" s="5"/>
+      <c r="CM1" s="5"/>
+      <c r="CN1" s="5"/>
+      <c r="CO1" s="5"/>
+      <c r="CP1" s="5"/>
+      <c r="CQ1" s="5"/>
+      <c r="CR1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="CS1" s="4"/>
-      <c r="CT1" s="4"/>
-      <c r="CU1" s="4"/>
-      <c r="CV1" s="4"/>
+      <c r="CS1" s="5"/>
+      <c r="CT1" s="5"/>
+      <c r="CU1" s="5"/>
+      <c r="CV1" s="5"/>
     </row>
     <row r="2" spans="1:102">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="4"/>
-      <c r="AP2" s="4"/>
-      <c r="AQ2" s="4"/>
-      <c r="AR2" s="4"/>
-      <c r="AS2" s="4" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AT2" s="4"/>
-      <c r="AU2" s="4"/>
-      <c r="AV2" s="4"/>
-      <c r="AW2" s="4"/>
-      <c r="AX2" s="4"/>
-      <c r="AY2" s="4"/>
-      <c r="AZ2" s="4"/>
-      <c r="BA2" s="4"/>
-      <c r="BB2" s="4"/>
-      <c r="BC2" s="4"/>
-      <c r="BD2" s="4"/>
-      <c r="BE2" s="4"/>
-      <c r="BF2" s="4"/>
-      <c r="BG2" s="4"/>
-      <c r="BH2" s="4"/>
-      <c r="BI2" s="4"/>
-      <c r="BJ2" s="4"/>
-      <c r="BK2" s="4"/>
-      <c r="BL2" s="4"/>
-      <c r="BM2" s="4"/>
-      <c r="BN2" s="4"/>
-      <c r="BO2" s="4"/>
-      <c r="BP2" s="4"/>
-      <c r="BQ2" s="4"/>
-      <c r="BR2" s="4"/>
-      <c r="BS2" s="4"/>
-      <c r="BT2" s="4"/>
-      <c r="BU2" s="4"/>
-      <c r="BV2" s="4"/>
-      <c r="BW2" s="4" t="s">
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="5"/>
+      <c r="BD2" s="5"/>
+      <c r="BE2" s="5"/>
+      <c r="BF2" s="5"/>
+      <c r="BG2" s="5"/>
+      <c r="BH2" s="5"/>
+      <c r="BI2" s="5"/>
+      <c r="BJ2" s="5"/>
+      <c r="BK2" s="5"/>
+      <c r="BL2" s="5"/>
+      <c r="BM2" s="5"/>
+      <c r="BN2" s="5"/>
+      <c r="BO2" s="5"/>
+      <c r="BP2" s="5"/>
+      <c r="BQ2" s="5"/>
+      <c r="BR2" s="5"/>
+      <c r="BS2" s="5"/>
+      <c r="BT2" s="5"/>
+      <c r="BU2" s="5"/>
+      <c r="BV2" s="5"/>
+      <c r="BW2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="BX2" s="4"/>
-      <c r="BY2" s="4"/>
-      <c r="BZ2" s="4"/>
-      <c r="CA2" s="4"/>
-      <c r="CB2" s="4"/>
-      <c r="CC2" s="4"/>
-      <c r="CD2" s="4"/>
-      <c r="CE2" s="4"/>
-      <c r="CF2" s="4"/>
-      <c r="CG2" s="4"/>
-      <c r="CH2" s="4"/>
-      <c r="CI2" s="4"/>
-      <c r="CJ2" s="4"/>
-      <c r="CK2" s="4"/>
-      <c r="CL2" s="4"/>
-      <c r="CM2" s="4"/>
-      <c r="CN2" s="4"/>
-      <c r="CO2" s="4"/>
-      <c r="CP2" s="4"/>
-      <c r="CQ2" s="4"/>
-      <c r="CR2" s="4"/>
-      <c r="CS2" s="4"/>
-      <c r="CT2" s="4"/>
-      <c r="CU2" s="4"/>
-      <c r="CV2" s="4"/>
+      <c r="BX2" s="5"/>
+      <c r="BY2" s="5"/>
+      <c r="BZ2" s="5"/>
+      <c r="CA2" s="5"/>
+      <c r="CB2" s="5"/>
+      <c r="CC2" s="5"/>
+      <c r="CD2" s="5"/>
+      <c r="CE2" s="5"/>
+      <c r="CF2" s="5"/>
+      <c r="CG2" s="5"/>
+      <c r="CH2" s="5"/>
+      <c r="CI2" s="5"/>
+      <c r="CJ2" s="5"/>
+      <c r="CK2" s="5"/>
+      <c r="CL2" s="5"/>
+      <c r="CM2" s="5"/>
+      <c r="CN2" s="5"/>
+      <c r="CO2" s="5"/>
+      <c r="CP2" s="5"/>
+      <c r="CQ2" s="5"/>
+      <c r="CR2" s="5"/>
+      <c r="CS2" s="5"/>
+      <c r="CT2" s="5"/>
+      <c r="CU2" s="5"/>
+      <c r="CV2" s="5"/>
     </row>
     <row r="3" spans="1:102">
       <c r="B3" s="1">
@@ -1360,13 +1400,8 @@
       <c r="CW4" s="1"/>
       <c r="CX4" s="1"/>
     </row>
-    <row r="5" spans="1:102">
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-    </row>
     <row r="6" spans="1:102">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="2"/>
@@ -1374,37 +1409,26 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
     </row>
     <row r="7" spans="1:102">
-      <c r="A7" s="9"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="8" spans="1:102">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2"/>
@@ -1412,9 +1436,9 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1422,43 +1446,28 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:102">
-      <c r="A9" s="9"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="A9" s="10"/>
     </row>
     <row r="10" spans="1:102">
-      <c r="A10" s="9">
-        <v>2.1</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="A10" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="I10" s="6"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1474,29 +1483,28 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="6"/>
     </row>
     <row r="11" spans="1:102">
-      <c r="A11" s="9"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="A11" s="10"/>
     </row>
     <row r="12" spans="1:102">
-      <c r="A12" s="9">
-        <v>2.2000000000000002</v>
-      </c>
+      <c r="A12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
@@ -1507,90 +1515,135 @@
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
       <c r="AM12" s="2"/>
-      <c r="AN12" s="2"/>
-      <c r="AO12" s="2"/>
-      <c r="AP12" s="2"/>
-      <c r="AQ12" s="2"/>
-      <c r="AR12" s="2"/>
-      <c r="AS12" s="2"/>
-      <c r="AT12" s="2"/>
-      <c r="AU12" s="2"/>
-      <c r="AV12" s="2"/>
-      <c r="AW12" s="2"/>
-      <c r="AX12" s="2"/>
-      <c r="AY12" s="2"/>
-      <c r="AZ12" s="2"/>
-      <c r="BA12" s="2"/>
-      <c r="BB12" s="2"/>
-      <c r="BC12" s="2"/>
-      <c r="BD12" s="2"/>
-      <c r="BE12" s="2"/>
-      <c r="BF12" s="2"/>
-      <c r="BG12" s="2"/>
-      <c r="BH12" s="2"/>
-      <c r="BI12" s="2"/>
-      <c r="BJ12" s="2"/>
-      <c r="BK12" s="2"/>
-      <c r="BL12" s="2"/>
-      <c r="BM12" s="2"/>
-      <c r="BN12" s="2"/>
-      <c r="BO12" s="2"/>
-      <c r="BP12" s="2"/>
-      <c r="BQ12" s="2"/>
-      <c r="BR12" s="2"/>
-      <c r="BS12" s="2"/>
-      <c r="BT12" s="2"/>
-      <c r="BU12" s="2"/>
-      <c r="BV12" s="2"/>
-      <c r="BW12" s="2"/>
-      <c r="BX12" s="2"/>
-      <c r="BY12" s="2"/>
-      <c r="BZ12" s="2"/>
-      <c r="CA12" s="2"/>
+      <c r="AN12" s="6"/>
+      <c r="AO12" s="6"/>
+      <c r="AP12" s="6"/>
+      <c r="AQ12" s="6"/>
+      <c r="AR12" s="6"/>
+      <c r="AS12" s="6"/>
+      <c r="AT12" s="6"/>
+      <c r="AU12" s="6"/>
+      <c r="AV12" s="6"/>
+      <c r="AW12" s="6"/>
+      <c r="AX12" s="6"/>
+      <c r="AY12" s="6"/>
+      <c r="AZ12" s="6"/>
+      <c r="BA12" s="6"/>
+      <c r="BB12" s="6"/>
+      <c r="BC12" s="6"/>
+      <c r="BD12" s="6"/>
+      <c r="BE12" s="6"/>
+      <c r="BF12" s="6"/>
+      <c r="BG12" s="6"/>
+      <c r="BH12" s="6"/>
+      <c r="BI12" s="6"/>
+      <c r="BJ12" s="6"/>
+      <c r="BK12" s="6"/>
+      <c r="BL12" s="6"/>
+      <c r="BM12" s="6"/>
+      <c r="BN12" s="6"/>
+      <c r="BO12" s="6"/>
+      <c r="BP12" s="6"/>
+      <c r="BQ12" s="6"/>
+      <c r="BR12" s="6"/>
+      <c r="BS12" s="6"/>
+      <c r="BT12" s="6"/>
+      <c r="BU12" s="6"/>
+      <c r="BV12" s="6"/>
+      <c r="BW12" s="6"/>
+      <c r="BX12" s="6"/>
+      <c r="BY12" s="6"/>
+      <c r="BZ12" s="6"/>
+      <c r="CA12" s="6"/>
+      <c r="CB12" s="6"/>
     </row>
     <row r="13" spans="1:102">
-      <c r="A13" s="9"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="7"/>
-      <c r="AE13" s="7"/>
-      <c r="AF13" s="7"/>
-      <c r="AG13" s="7"/>
-      <c r="AH13" s="7"/>
-      <c r="AI13" s="7"/>
-      <c r="AJ13" s="7"/>
-      <c r="AK13" s="7"/>
-      <c r="AL13" s="7"/>
-      <c r="AM13" s="7"/>
-      <c r="AN13" s="7"/>
-      <c r="AO13" s="7"/>
-      <c r="AP13" s="7"/>
+      <c r="A13" s="10"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6"/>
+      <c r="AJ13" s="6"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="6"/>
+      <c r="AP13" s="6"/>
+      <c r="AQ13" s="6"/>
+      <c r="AR13" s="6"/>
+      <c r="AS13" s="6"/>
+      <c r="AT13" s="6"/>
+      <c r="AU13" s="6"/>
+      <c r="AV13" s="6"/>
+      <c r="AW13" s="6"/>
+      <c r="AX13" s="6"/>
+      <c r="AY13" s="6"/>
+      <c r="AZ13" s="6"/>
+      <c r="BA13" s="6"/>
+      <c r="BB13" s="6"/>
+      <c r="BC13" s="6"/>
+      <c r="BD13" s="6"/>
+      <c r="BE13" s="6"/>
+      <c r="BF13" s="6"/>
+      <c r="BG13" s="6"/>
+      <c r="BH13" s="6"/>
+      <c r="BI13" s="6"/>
+      <c r="BJ13" s="6"/>
+      <c r="BK13" s="6"/>
+      <c r="BL13" s="6"/>
+      <c r="BM13" s="6"/>
+      <c r="BN13" s="6"/>
+      <c r="BO13" s="6"/>
+      <c r="BP13" s="6"/>
+      <c r="BQ13" s="6"/>
+      <c r="BR13" s="6"/>
+      <c r="BS13" s="6"/>
+      <c r="BT13" s="6"/>
+      <c r="BU13" s="6"/>
+      <c r="BV13" s="6"/>
+      <c r="BW13" s="6"/>
+      <c r="BX13" s="6"/>
+      <c r="BY13" s="6"/>
+      <c r="BZ13" s="6"/>
+      <c r="CA13" s="6"/>
+      <c r="CB13" s="6"/>
+      <c r="CC13" s="6"/>
+      <c r="CD13" s="6"/>
+      <c r="CE13" s="6"/>
+      <c r="CF13" s="6"/>
+      <c r="CG13" s="6"/>
+      <c r="CH13" s="6"/>
     </row>
     <row r="14" spans="1:102">
-      <c r="A14" s="9">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H14" s="7"/>
+      <c r="A14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="6"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -1612,84 +1665,172 @@
       <c r="AA14" s="8"/>
       <c r="AB14" s="8"/>
       <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="7"/>
-      <c r="AF14" s="7"/>
-      <c r="AG14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="7"/>
-      <c r="AJ14" s="7"/>
-      <c r="AK14" s="7"/>
-      <c r="AL14" s="7"/>
-      <c r="AM14" s="7"/>
-      <c r="AN14" s="7"/>
-      <c r="AO14" s="7"/>
-      <c r="AP14" s="7"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
+      <c r="AP14" s="6"/>
+      <c r="AQ14" s="6"/>
+      <c r="AR14" s="6"/>
+      <c r="AS14" s="6"/>
+      <c r="AT14" s="6"/>
+      <c r="AU14" s="6"/>
+      <c r="AV14" s="6"/>
+      <c r="AW14" s="6"/>
+      <c r="AX14" s="6"/>
+      <c r="AY14" s="6"/>
+      <c r="AZ14" s="6"/>
+      <c r="BA14" s="6"/>
+      <c r="BB14" s="6"/>
+      <c r="BC14" s="6"/>
+      <c r="BD14" s="6"/>
+      <c r="BE14" s="6"/>
+      <c r="BF14" s="6"/>
+      <c r="BG14" s="6"/>
+      <c r="BH14" s="6"/>
+      <c r="BI14" s="6"/>
+      <c r="BJ14" s="6"/>
+      <c r="BK14" s="6"/>
+      <c r="BL14" s="6"/>
+      <c r="BM14" s="6"/>
+      <c r="BN14" s="6"/>
+      <c r="BO14" s="6"/>
+      <c r="BP14" s="6"/>
+      <c r="BQ14" s="6"/>
+      <c r="BR14" s="6"/>
+      <c r="BS14" s="6"/>
+      <c r="BT14" s="6"/>
+      <c r="BU14" s="6"/>
+      <c r="BV14" s="6"/>
+      <c r="BW14" s="6"/>
+      <c r="BX14" s="6"/>
+      <c r="BY14" s="6"/>
+      <c r="BZ14" s="6"/>
+      <c r="CA14" s="6"/>
+      <c r="CB14" s="6"/>
+      <c r="CC14" s="6"/>
+      <c r="CD14" s="6"/>
+      <c r="CE14" s="6"/>
+      <c r="CF14" s="6"/>
+      <c r="CG14" s="6"/>
+      <c r="CH14" s="6"/>
     </row>
     <row r="15" spans="1:102">
-      <c r="A15" s="9"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="7"/>
-      <c r="AE15" s="7"/>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="7"/>
-      <c r="AH15" s="7"/>
-      <c r="AI15" s="7"/>
-      <c r="AJ15" s="7"/>
-      <c r="AK15" s="7"/>
-      <c r="AL15" s="7"/>
-      <c r="AM15" s="7"/>
-      <c r="AN15" s="7"/>
-      <c r="AO15" s="7"/>
-      <c r="AP15" s="7"/>
+      <c r="A15" s="10"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="6"/>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="6"/>
+      <c r="AL15" s="6"/>
+      <c r="AM15" s="6"/>
+      <c r="AN15" s="6"/>
+      <c r="AO15" s="6"/>
+      <c r="AP15" s="6"/>
+      <c r="AQ15" s="6"/>
+      <c r="AR15" s="6"/>
+      <c r="AS15" s="6"/>
+      <c r="AT15" s="6"/>
+      <c r="AU15" s="6"/>
+      <c r="AV15" s="6"/>
+      <c r="AW15" s="6"/>
+      <c r="AX15" s="6"/>
+      <c r="AY15" s="6"/>
+      <c r="AZ15" s="6"/>
+      <c r="BA15" s="6"/>
+      <c r="BB15" s="6"/>
+      <c r="BC15" s="6"/>
+      <c r="BD15" s="6"/>
+      <c r="BE15" s="6"/>
+      <c r="BF15" s="6"/>
+      <c r="BG15" s="6"/>
+      <c r="BH15" s="6"/>
+      <c r="BI15" s="6"/>
+      <c r="BJ15" s="6"/>
+      <c r="BK15" s="6"/>
+      <c r="BL15" s="6"/>
+      <c r="BM15" s="6"/>
+      <c r="BN15" s="6"/>
+      <c r="BO15" s="6"/>
+      <c r="BP15" s="6"/>
+      <c r="BQ15" s="6"/>
+      <c r="BR15" s="6"/>
+      <c r="BS15" s="6"/>
+      <c r="BT15" s="6"/>
+      <c r="BU15" s="6"/>
+      <c r="BV15" s="6"/>
+      <c r="BW15" s="6"/>
+      <c r="BX15" s="6"/>
+      <c r="BY15" s="6"/>
+      <c r="BZ15" s="6"/>
+      <c r="CA15" s="6"/>
+      <c r="CB15" s="6"/>
+      <c r="CC15" s="6"/>
+      <c r="CD15" s="6"/>
+      <c r="CE15" s="6"/>
+      <c r="CF15" s="6"/>
+      <c r="CG15" s="6"/>
+      <c r="CH15" s="6"/>
     </row>
     <row r="16" spans="1:102">
-      <c r="A16" s="9">
-        <v>2.4</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="7"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="7"/>
+      <c r="A16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
@@ -1733,58 +1874,144 @@
       <c r="BR16" s="2"/>
       <c r="BS16" s="2"/>
       <c r="BT16" s="2"/>
-      <c r="BU16" s="2"/>
-      <c r="BV16" s="2"/>
-      <c r="BW16" s="2"/>
-      <c r="BX16" s="2"/>
-      <c r="BY16" s="2"/>
-      <c r="BZ16" s="2"/>
-      <c r="CA16" s="2"/>
-      <c r="CB16" s="2"/>
-      <c r="CC16" s="2"/>
-      <c r="CD16" s="2"/>
-      <c r="CE16" s="2"/>
-      <c r="CF16" s="2"/>
-      <c r="CG16" s="2"/>
-      <c r="CH16" s="2"/>
-      <c r="CI16" s="7"/>
-      <c r="CJ16" s="7"/>
-      <c r="CK16" s="7"/>
-      <c r="CL16" s="7"/>
-      <c r="CM16" s="7"/>
-      <c r="CN16" s="7"/>
-      <c r="CO16" s="7"/>
-      <c r="CP16" s="7"/>
-      <c r="CQ16" s="7"/>
-    </row>
-    <row r="17" spans="1:100">
-      <c r="A17" s="9"/>
-    </row>
-    <row r="18" spans="1:100">
-      <c r="A18" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="2"/>
+      <c r="BU16" s="6"/>
+      <c r="BV16" s="6"/>
+      <c r="BW16" s="6"/>
+      <c r="BX16" s="6"/>
+      <c r="BY16" s="6"/>
+      <c r="BZ16" s="6"/>
+      <c r="CA16" s="6"/>
+      <c r="CB16" s="6"/>
+      <c r="CC16" s="6"/>
+      <c r="CD16" s="6"/>
+      <c r="CE16" s="6"/>
+      <c r="CF16" s="6"/>
+      <c r="CG16" s="6"/>
+      <c r="CH16" s="6"/>
+    </row>
+    <row r="17" spans="1:101">
+      <c r="A17" s="10"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="6"/>
+      <c r="AK17" s="6"/>
+      <c r="AL17" s="6"/>
+      <c r="AM17" s="6"/>
+      <c r="AN17" s="6"/>
+      <c r="AO17" s="6"/>
+      <c r="AP17" s="6"/>
+      <c r="AQ17" s="6"/>
+      <c r="AR17" s="6"/>
+      <c r="AS17" s="6"/>
+      <c r="AT17" s="6"/>
+      <c r="AU17" s="6"/>
+      <c r="AV17" s="6"/>
+      <c r="AW17" s="6"/>
+      <c r="AX17" s="6"/>
+      <c r="AY17" s="6"/>
+      <c r="AZ17" s="6"/>
+      <c r="BA17" s="6"/>
+      <c r="BB17" s="6"/>
+      <c r="BC17" s="6"/>
+      <c r="BD17" s="6"/>
+      <c r="BE17" s="6"/>
+      <c r="BF17" s="6"/>
+      <c r="BG17" s="6"/>
+      <c r="BH17" s="6"/>
+      <c r="BI17" s="6"/>
+      <c r="BJ17" s="6"/>
+      <c r="BK17" s="6"/>
+      <c r="BL17" s="6"/>
+      <c r="BM17" s="6"/>
+      <c r="BN17" s="6"/>
+      <c r="BO17" s="6"/>
+      <c r="BP17" s="6"/>
+      <c r="BQ17" s="6"/>
+      <c r="BR17" s="6"/>
+      <c r="BS17" s="6"/>
+      <c r="BT17" s="6"/>
+      <c r="BU17" s="6"/>
+      <c r="BV17" s="6"/>
+      <c r="BW17" s="6"/>
+      <c r="BX17" s="6"/>
+      <c r="BY17" s="6"/>
+      <c r="BZ17" s="6"/>
+      <c r="CA17" s="6"/>
+      <c r="CB17" s="6"/>
+      <c r="CC17" s="6"/>
+      <c r="CD17" s="6"/>
+      <c r="CE17" s="6"/>
+      <c r="CF17" s="6"/>
+      <c r="CG17" s="6"/>
+      <c r="CH17" s="6"/>
+      <c r="CI17" s="6"/>
+      <c r="CJ17" s="6"/>
+      <c r="CK17" s="6"/>
+      <c r="CL17" s="6"/>
+      <c r="CM17" s="6"/>
+      <c r="CN17" s="6"/>
+      <c r="CO17" s="6"/>
+      <c r="CP17" s="6"/>
+      <c r="CQ17" s="6"/>
+      <c r="CR17" s="6"/>
+      <c r="CS17" s="6"/>
+      <c r="CT17" s="6"/>
+      <c r="CU17" s="6"/>
+      <c r="CV17" s="6"/>
+      <c r="CW17" s="7"/>
+    </row>
+    <row r="18" spans="1:101">
+      <c r="A18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
       <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
@@ -1800,88 +2027,218 @@
       <c r="AP18" s="2"/>
       <c r="AQ18" s="2"/>
       <c r="AR18" s="2"/>
-      <c r="AS18" s="7"/>
-      <c r="AT18" s="7"/>
-      <c r="AU18" s="7"/>
-      <c r="AV18" s="7"/>
-      <c r="AW18" s="7"/>
-      <c r="AX18" s="7"/>
-      <c r="AY18" s="7"/>
-      <c r="AZ18" s="7"/>
-      <c r="BA18" s="7"/>
-      <c r="BB18" s="7"/>
-      <c r="BC18" s="7"/>
-      <c r="BD18" s="7"/>
-      <c r="BE18" s="7"/>
-      <c r="BF18" s="7"/>
-      <c r="BG18" s="7"/>
-      <c r="BH18" s="7"/>
-      <c r="BI18" s="7"/>
-      <c r="BJ18" s="7"/>
-      <c r="BK18" s="7"/>
-      <c r="BL18" s="7"/>
-      <c r="BM18" s="7"/>
-      <c r="BN18" s="7"/>
-    </row>
-    <row r="19" spans="1:100">
-      <c r="A19" s="9"/>
-    </row>
-    <row r="20" spans="1:100">
-      <c r="A20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="2"/>
-      <c r="AD20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="2"/>
-      <c r="AH20" s="2"/>
-      <c r="AI20" s="2"/>
-      <c r="AJ20" s="2"/>
-      <c r="AK20" s="2"/>
-      <c r="AL20" s="2"/>
-      <c r="AM20" s="2"/>
-      <c r="AN20" s="2"/>
-      <c r="AO20" s="2"/>
-      <c r="AP20" s="2"/>
-      <c r="AQ20" s="2"/>
-      <c r="AR20" s="2"/>
-      <c r="AS20" s="2"/>
-      <c r="AT20" s="2"/>
-      <c r="AU20" s="2"/>
-      <c r="AV20" s="2"/>
-      <c r="AW20" s="2"/>
-      <c r="AX20" s="2"/>
-      <c r="AY20" s="2"/>
-      <c r="AZ20" s="2"/>
-      <c r="BA20" s="2"/>
-      <c r="BB20" s="2"/>
-      <c r="BC20" s="2"/>
-      <c r="BD20" s="2"/>
-      <c r="BE20" s="2"/>
-      <c r="BF20" s="2"/>
-      <c r="BG20" s="2"/>
-      <c r="BH20" s="2"/>
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="2"/>
+      <c r="AU18" s="2"/>
+      <c r="AV18" s="2"/>
+      <c r="AW18" s="2"/>
+      <c r="AX18" s="2"/>
+      <c r="AY18" s="2"/>
+      <c r="AZ18" s="2"/>
+      <c r="BA18" s="2"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="2"/>
+      <c r="BD18" s="2"/>
+      <c r="BE18" s="2"/>
+      <c r="BF18" s="2"/>
+      <c r="BG18" s="2"/>
+      <c r="BH18" s="2"/>
+      <c r="BI18" s="2"/>
+      <c r="BJ18" s="2"/>
+      <c r="BK18" s="2"/>
+      <c r="BL18" s="2"/>
+      <c r="BM18" s="2"/>
+      <c r="BN18" s="2"/>
+      <c r="BO18" s="2"/>
+      <c r="BP18" s="6"/>
+      <c r="BQ18" s="6"/>
+      <c r="BR18" s="6"/>
+      <c r="BS18" s="6"/>
+      <c r="BT18" s="6"/>
+      <c r="BU18" s="6"/>
+      <c r="BV18" s="6"/>
+      <c r="BW18" s="6"/>
+      <c r="BX18" s="6"/>
+      <c r="BY18" s="6"/>
+      <c r="BZ18" s="6"/>
+      <c r="CA18" s="6"/>
+      <c r="CB18" s="6"/>
+      <c r="CC18" s="6"/>
+      <c r="CD18" s="6"/>
+      <c r="CE18" s="6"/>
+      <c r="CF18" s="6"/>
+      <c r="CG18" s="6"/>
+      <c r="CH18" s="6"/>
+      <c r="CI18" s="6"/>
+      <c r="CJ18" s="6"/>
+      <c r="CK18" s="6"/>
+      <c r="CL18" s="6"/>
+      <c r="CM18" s="6"/>
+      <c r="CN18" s="6"/>
+      <c r="CO18" s="6"/>
+      <c r="CP18" s="6"/>
+      <c r="CQ18" s="6"/>
+      <c r="CR18" s="6"/>
+      <c r="CS18" s="6"/>
+      <c r="CT18" s="6"/>
+      <c r="CU18" s="6"/>
+      <c r="CV18" s="6"/>
+      <c r="CW18" s="7"/>
+    </row>
+    <row r="19" spans="1:101">
+      <c r="A19" s="10"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6"/>
+      <c r="AG19" s="6"/>
+      <c r="AH19" s="6"/>
+      <c r="AI19" s="6"/>
+      <c r="AJ19" s="6"/>
+      <c r="AK19" s="6"/>
+      <c r="AL19" s="6"/>
+      <c r="AM19" s="6"/>
+      <c r="AN19" s="6"/>
+      <c r="AO19" s="6"/>
+      <c r="AP19" s="6"/>
+      <c r="AQ19" s="6"/>
+      <c r="AR19" s="6"/>
+      <c r="AS19" s="6"/>
+      <c r="AT19" s="6"/>
+      <c r="AU19" s="6"/>
+      <c r="AV19" s="6"/>
+      <c r="AW19" s="6"/>
+      <c r="AX19" s="6"/>
+      <c r="AY19" s="6"/>
+      <c r="AZ19" s="6"/>
+      <c r="BA19" s="6"/>
+      <c r="BB19" s="6"/>
+      <c r="BC19" s="6"/>
+      <c r="BD19" s="6"/>
+      <c r="BE19" s="6"/>
+      <c r="BF19" s="6"/>
+      <c r="BG19" s="6"/>
+      <c r="BH19" s="6"/>
+      <c r="BI19" s="6"/>
+      <c r="BJ19" s="6"/>
+      <c r="BK19" s="6"/>
+      <c r="BL19" s="6"/>
+      <c r="BM19" s="6"/>
+      <c r="BN19" s="6"/>
+      <c r="BO19" s="6"/>
+      <c r="BP19" s="6"/>
+      <c r="BQ19" s="6"/>
+      <c r="BR19" s="6"/>
+      <c r="BS19" s="6"/>
+      <c r="BT19" s="6"/>
+      <c r="BU19" s="6"/>
+      <c r="BV19" s="6"/>
+      <c r="BW19" s="6"/>
+      <c r="BX19" s="6"/>
+      <c r="BY19" s="6"/>
+      <c r="BZ19" s="6"/>
+      <c r="CA19" s="6"/>
+      <c r="CB19" s="6"/>
+      <c r="CC19" s="6"/>
+      <c r="CD19" s="6"/>
+      <c r="CE19" s="6"/>
+      <c r="CF19" s="6"/>
+      <c r="CG19" s="6"/>
+      <c r="CH19" s="6"/>
+      <c r="CI19" s="6"/>
+      <c r="CJ19" s="6"/>
+      <c r="CK19" s="6"/>
+      <c r="CL19" s="6"/>
+      <c r="CM19" s="6"/>
+      <c r="CN19" s="6"/>
+      <c r="CO19" s="6"/>
+      <c r="CP19" s="6"/>
+      <c r="CQ19" s="6"/>
+      <c r="CR19" s="6"/>
+      <c r="CS19" s="6"/>
+      <c r="CT19" s="6"/>
+      <c r="CU19" s="6"/>
+      <c r="CV19" s="6"/>
+      <c r="CW19" s="7"/>
+    </row>
+    <row r="20" spans="1:101">
+      <c r="A20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="6"/>
+      <c r="AK20" s="6"/>
+      <c r="AL20" s="6"/>
+      <c r="AM20" s="6"/>
+      <c r="AN20" s="6"/>
+      <c r="AO20" s="6"/>
+      <c r="AP20" s="6"/>
+      <c r="AQ20" s="6"/>
+      <c r="AR20" s="6"/>
+      <c r="AS20" s="6"/>
+      <c r="AT20" s="6"/>
+      <c r="AU20" s="6"/>
+      <c r="AV20" s="6"/>
+      <c r="AW20" s="6"/>
+      <c r="AX20" s="6"/>
+      <c r="AY20" s="6"/>
+      <c r="AZ20" s="6"/>
+      <c r="BA20" s="6"/>
+      <c r="BB20" s="6"/>
+      <c r="BC20" s="6"/>
+      <c r="BD20" s="6"/>
+      <c r="BE20" s="6"/>
+      <c r="BF20" s="6"/>
+      <c r="BG20" s="6"/>
+      <c r="BH20" s="6"/>
       <c r="BI20" s="2"/>
       <c r="BJ20" s="2"/>
       <c r="BK20" s="2"/>
@@ -1894,37 +2251,980 @@
       <c r="BR20" s="2"/>
       <c r="BS20" s="2"/>
       <c r="BT20" s="2"/>
-      <c r="BU20" s="2"/>
-      <c r="BV20" s="2"/>
-      <c r="BW20" s="2"/>
-      <c r="BX20" s="2"/>
-      <c r="BY20" s="2"/>
-      <c r="BZ20" s="2"/>
-      <c r="CA20" s="2"/>
-      <c r="CB20" s="2"/>
-      <c r="CC20" s="2"/>
-      <c r="CD20" s="2"/>
-      <c r="CE20" s="2"/>
-      <c r="CF20" s="2"/>
-      <c r="CG20" s="2"/>
-      <c r="CH20" s="2"/>
-      <c r="CI20" s="2"/>
-      <c r="CJ20" s="2"/>
-      <c r="CK20" s="2"/>
-      <c r="CL20" s="2"/>
-      <c r="CM20" s="2"/>
-      <c r="CN20" s="2"/>
-      <c r="CO20" s="2"/>
-      <c r="CP20" s="2"/>
-      <c r="CQ20" s="2"/>
-      <c r="CR20" s="2"/>
-      <c r="CS20" s="2"/>
-      <c r="CT20" s="2"/>
-      <c r="CU20" s="2"/>
-      <c r="CV20" s="2"/>
+      <c r="BU20" s="6"/>
+      <c r="BV20" s="6"/>
+      <c r="BW20" s="6"/>
+      <c r="BX20" s="6"/>
+      <c r="BY20" s="6"/>
+      <c r="BZ20" s="6"/>
+      <c r="CA20" s="6"/>
+      <c r="CB20" s="6"/>
+      <c r="CC20" s="6"/>
+      <c r="CD20" s="6"/>
+      <c r="CE20" s="6"/>
+      <c r="CF20" s="6"/>
+      <c r="CG20" s="6"/>
+      <c r="CH20" s="6"/>
+      <c r="CI20" s="6"/>
+      <c r="CJ20" s="6"/>
+      <c r="CK20" s="6"/>
+      <c r="CL20" s="6"/>
+      <c r="CM20" s="6"/>
+      <c r="CN20" s="6"/>
+      <c r="CO20" s="6"/>
+      <c r="CP20" s="6"/>
+      <c r="CQ20" s="6"/>
+      <c r="CR20" s="6"/>
+      <c r="CS20" s="6"/>
+      <c r="CT20" s="6"/>
+      <c r="CU20" s="6"/>
+      <c r="CV20" s="6"/>
+      <c r="CW20" s="7"/>
+    </row>
+    <row r="21" spans="1:101">
+      <c r="A21" s="10"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6"/>
+      <c r="AI21" s="6"/>
+      <c r="AJ21" s="6"/>
+      <c r="AK21" s="6"/>
+      <c r="AL21" s="6"/>
+      <c r="AM21" s="6"/>
+      <c r="AN21" s="6"/>
+      <c r="AO21" s="6"/>
+      <c r="AP21" s="6"/>
+      <c r="AQ21" s="6"/>
+      <c r="AR21" s="6"/>
+      <c r="AS21" s="6"/>
+      <c r="AT21" s="6"/>
+      <c r="AU21" s="6"/>
+      <c r="AV21" s="6"/>
+      <c r="AW21" s="6"/>
+      <c r="AX21" s="6"/>
+      <c r="AY21" s="6"/>
+      <c r="AZ21" s="6"/>
+      <c r="BA21" s="6"/>
+      <c r="BB21" s="6"/>
+      <c r="BC21" s="6"/>
+      <c r="BD21" s="6"/>
+      <c r="BE21" s="6"/>
+      <c r="BF21" s="6"/>
+      <c r="BG21" s="6"/>
+      <c r="BH21" s="6"/>
+      <c r="BI21" s="6"/>
+      <c r="BJ21" s="6"/>
+      <c r="BK21" s="6"/>
+      <c r="BL21" s="6"/>
+      <c r="BM21" s="6"/>
+      <c r="BN21" s="6"/>
+      <c r="BO21" s="6"/>
+      <c r="BP21" s="6"/>
+      <c r="BQ21" s="6"/>
+      <c r="BR21" s="6"/>
+      <c r="BS21" s="6"/>
+      <c r="BT21" s="6"/>
+      <c r="BU21" s="6"/>
+      <c r="BV21" s="6"/>
+      <c r="BW21" s="6"/>
+      <c r="BX21" s="6"/>
+      <c r="BY21" s="6"/>
+      <c r="BZ21" s="6"/>
+      <c r="CA21" s="6"/>
+      <c r="CB21" s="6"/>
+      <c r="CC21" s="6"/>
+      <c r="CD21" s="6"/>
+      <c r="CE21" s="6"/>
+      <c r="CF21" s="6"/>
+      <c r="CG21" s="6"/>
+      <c r="CH21" s="6"/>
+      <c r="CI21" s="6"/>
+      <c r="CJ21" s="6"/>
+      <c r="CK21" s="6"/>
+      <c r="CL21" s="6"/>
+      <c r="CM21" s="6"/>
+      <c r="CN21" s="6"/>
+      <c r="CO21" s="6"/>
+      <c r="CP21" s="6"/>
+      <c r="CQ21" s="6"/>
+      <c r="CR21" s="6"/>
+      <c r="CS21" s="6"/>
+      <c r="CT21" s="6"/>
+      <c r="CU21" s="6"/>
+      <c r="CV21" s="6"/>
+      <c r="CW21" s="7"/>
+    </row>
+    <row r="22" spans="1:101">
+      <c r="A22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6"/>
+      <c r="AE22" s="6"/>
+      <c r="AF22" s="6"/>
+      <c r="AG22" s="6"/>
+      <c r="AH22" s="6"/>
+      <c r="AI22" s="6"/>
+      <c r="AJ22" s="6"/>
+      <c r="AK22" s="6"/>
+      <c r="AL22" s="6"/>
+      <c r="AM22" s="6"/>
+      <c r="AN22" s="6"/>
+      <c r="AO22" s="6"/>
+      <c r="AP22" s="6"/>
+      <c r="AQ22" s="6"/>
+      <c r="AR22" s="6"/>
+      <c r="AS22" s="6"/>
+      <c r="AT22" s="6"/>
+      <c r="AU22" s="6"/>
+      <c r="AV22" s="6"/>
+      <c r="AW22" s="6"/>
+      <c r="AX22" s="6"/>
+      <c r="AY22" s="6"/>
+      <c r="AZ22" s="6"/>
+      <c r="BA22" s="6"/>
+      <c r="BB22" s="6"/>
+      <c r="BC22" s="6"/>
+      <c r="BD22" s="6"/>
+      <c r="BE22" s="6"/>
+      <c r="BF22" s="6"/>
+      <c r="BG22" s="6"/>
+      <c r="BH22" s="6"/>
+      <c r="BI22" s="6"/>
+      <c r="BJ22" s="6"/>
+      <c r="BK22" s="6"/>
+      <c r="BL22" s="6"/>
+      <c r="BM22" s="6"/>
+      <c r="BN22" s="6"/>
+      <c r="BO22" s="6"/>
+      <c r="BP22" s="6"/>
+      <c r="BQ22" s="6"/>
+      <c r="BR22" s="6"/>
+      <c r="BS22" s="6"/>
+      <c r="BT22" s="6"/>
+      <c r="BU22" s="2"/>
+      <c r="BV22" s="2"/>
+      <c r="BW22" s="2"/>
+      <c r="BX22" s="2"/>
+      <c r="BY22" s="2"/>
+      <c r="BZ22" s="2"/>
+      <c r="CA22" s="2"/>
+      <c r="CB22" s="2"/>
+      <c r="CC22" s="2"/>
+      <c r="CD22" s="6"/>
+      <c r="CE22" s="6"/>
+      <c r="CF22" s="6"/>
+      <c r="CG22" s="6"/>
+      <c r="CH22" s="6"/>
+      <c r="CI22" s="6"/>
+      <c r="CJ22" s="6"/>
+      <c r="CK22" s="6"/>
+      <c r="CL22" s="6"/>
+      <c r="CM22" s="6"/>
+      <c r="CN22" s="6"/>
+      <c r="CO22" s="6"/>
+      <c r="CP22" s="6"/>
+      <c r="CQ22" s="6"/>
+      <c r="CR22" s="6"/>
+      <c r="CS22" s="6"/>
+      <c r="CT22" s="6"/>
+      <c r="CU22" s="6"/>
+      <c r="CV22" s="6"/>
+      <c r="CW22" s="7"/>
+    </row>
+    <row r="23" spans="1:101">
+      <c r="A23" s="10"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="6"/>
+      <c r="AI23" s="6"/>
+      <c r="AJ23" s="6"/>
+      <c r="AK23" s="6"/>
+      <c r="AL23" s="6"/>
+      <c r="AM23" s="6"/>
+      <c r="AN23" s="6"/>
+      <c r="AO23" s="6"/>
+      <c r="AP23" s="6"/>
+      <c r="AQ23" s="6"/>
+      <c r="AR23" s="6"/>
+      <c r="AS23" s="6"/>
+      <c r="AT23" s="6"/>
+      <c r="AU23" s="6"/>
+      <c r="AV23" s="6"/>
+      <c r="AW23" s="6"/>
+      <c r="AX23" s="6"/>
+      <c r="AY23" s="6"/>
+      <c r="AZ23" s="6"/>
+      <c r="BA23" s="6"/>
+      <c r="BB23" s="6"/>
+      <c r="BC23" s="6"/>
+      <c r="BD23" s="6"/>
+      <c r="BE23" s="6"/>
+      <c r="BF23" s="6"/>
+      <c r="BG23" s="6"/>
+      <c r="BH23" s="6"/>
+      <c r="BI23" s="6"/>
+      <c r="BJ23" s="6"/>
+      <c r="BK23" s="6"/>
+      <c r="BL23" s="6"/>
+      <c r="BM23" s="6"/>
+      <c r="BN23" s="6"/>
+      <c r="BO23" s="6"/>
+      <c r="BP23" s="6"/>
+      <c r="BQ23" s="6"/>
+      <c r="BR23" s="6"/>
+      <c r="BS23" s="6"/>
+      <c r="BT23" s="6"/>
+      <c r="BU23" s="6"/>
+      <c r="BV23" s="6"/>
+      <c r="BW23" s="6"/>
+      <c r="BX23" s="6"/>
+      <c r="BY23" s="6"/>
+      <c r="BZ23" s="6"/>
+      <c r="CA23" s="6"/>
+      <c r="CB23" s="6"/>
+      <c r="CC23" s="6"/>
+      <c r="CD23" s="6"/>
+      <c r="CE23" s="6"/>
+      <c r="CF23" s="6"/>
+      <c r="CG23" s="6"/>
+      <c r="CH23" s="6"/>
+    </row>
+    <row r="24" spans="1:101">
+      <c r="A24" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
+      <c r="AH24" s="6"/>
+      <c r="AI24" s="6"/>
+      <c r="AJ24" s="6"/>
+      <c r="AK24" s="6"/>
+      <c r="AL24" s="6"/>
+      <c r="AM24" s="6"/>
+      <c r="AN24" s="6"/>
+      <c r="AO24" s="6"/>
+      <c r="AP24" s="6"/>
+      <c r="AQ24" s="6"/>
+      <c r="AR24" s="6"/>
+      <c r="AS24" s="6"/>
+      <c r="AT24" s="6"/>
+      <c r="AU24" s="6"/>
+      <c r="AV24" s="6"/>
+      <c r="AW24" s="6"/>
+      <c r="AX24" s="6"/>
+      <c r="AY24" s="6"/>
+      <c r="AZ24" s="6"/>
+      <c r="BA24" s="6"/>
+      <c r="BB24" s="6"/>
+      <c r="BC24" s="6"/>
+      <c r="BD24" s="6"/>
+      <c r="BE24" s="6"/>
+      <c r="BF24" s="6"/>
+      <c r="BG24" s="6"/>
+      <c r="BH24" s="6"/>
+      <c r="BI24" s="6"/>
+      <c r="BJ24" s="6"/>
+      <c r="BK24" s="6"/>
+      <c r="BL24" s="6"/>
+      <c r="BM24" s="6"/>
+      <c r="BN24" s="6"/>
+      <c r="BO24" s="6"/>
+      <c r="BP24" s="6"/>
+      <c r="BQ24" s="6"/>
+      <c r="BR24" s="6"/>
+      <c r="BS24" s="6"/>
+      <c r="BT24" s="6"/>
+      <c r="BU24" s="6"/>
+      <c r="BV24" s="6"/>
+      <c r="BW24" s="6"/>
+      <c r="BX24" s="6"/>
+      <c r="BY24" s="6"/>
+      <c r="BZ24" s="6"/>
+      <c r="CA24" s="2"/>
+      <c r="CB24" s="2"/>
+      <c r="CC24" s="2"/>
+      <c r="CD24" s="2"/>
+      <c r="CE24" s="2"/>
+      <c r="CF24" s="2"/>
+      <c r="CG24" s="2"/>
+      <c r="CH24" s="2"/>
+      <c r="CI24" s="2"/>
+      <c r="CJ24" s="2"/>
+      <c r="CK24" s="2"/>
+      <c r="CL24" s="2"/>
+      <c r="CM24" s="2"/>
+      <c r="CN24" s="2"/>
+    </row>
+    <row r="25" spans="1:101">
+      <c r="A25" s="10"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6"/>
+      <c r="AG25" s="6"/>
+      <c r="AH25" s="6"/>
+      <c r="AI25" s="6"/>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="6"/>
+      <c r="AL25" s="6"/>
+      <c r="AM25" s="6"/>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="6"/>
+      <c r="AP25" s="6"/>
+      <c r="AQ25" s="6"/>
+      <c r="AR25" s="6"/>
+      <c r="AS25" s="6"/>
+      <c r="AT25" s="6"/>
+      <c r="AU25" s="6"/>
+      <c r="AV25" s="6"/>
+      <c r="AW25" s="6"/>
+      <c r="AX25" s="6"/>
+      <c r="AY25" s="6"/>
+      <c r="AZ25" s="6"/>
+      <c r="BA25" s="6"/>
+      <c r="BB25" s="6"/>
+      <c r="BC25" s="6"/>
+      <c r="BD25" s="6"/>
+      <c r="BE25" s="6"/>
+      <c r="BF25" s="6"/>
+      <c r="BG25" s="6"/>
+      <c r="BH25" s="6"/>
+      <c r="BI25" s="6"/>
+      <c r="BJ25" s="6"/>
+      <c r="BK25" s="6"/>
+      <c r="BL25" s="6"/>
+      <c r="BM25" s="6"/>
+      <c r="BN25" s="6"/>
+      <c r="BO25" s="6"/>
+      <c r="BP25" s="6"/>
+      <c r="BQ25" s="6"/>
+      <c r="BR25" s="6"/>
+      <c r="BS25" s="6"/>
+      <c r="BT25" s="6"/>
+      <c r="BU25" s="6"/>
+      <c r="BV25" s="6"/>
+      <c r="BW25" s="6"/>
+      <c r="BX25" s="6"/>
+      <c r="BY25" s="6"/>
+      <c r="BZ25" s="6"/>
+      <c r="CA25" s="6"/>
+      <c r="CB25" s="6"/>
+      <c r="CC25" s="6"/>
+      <c r="CD25" s="6"/>
+      <c r="CE25" s="6"/>
+      <c r="CF25" s="6"/>
+      <c r="CG25" s="6"/>
+      <c r="CH25" s="6"/>
+    </row>
+    <row r="26" spans="1:101">
+      <c r="A26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="6"/>
+      <c r="AG26" s="6"/>
+      <c r="AH26" s="6"/>
+      <c r="AI26" s="6"/>
+      <c r="AJ26" s="6"/>
+      <c r="AK26" s="6"/>
+      <c r="AL26" s="6"/>
+      <c r="AM26" s="6"/>
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="6"/>
+      <c r="AP26" s="6"/>
+      <c r="AQ26" s="6"/>
+      <c r="AR26" s="6"/>
+      <c r="AS26" s="6"/>
+      <c r="AT26" s="6"/>
+      <c r="AU26" s="6"/>
+      <c r="AV26" s="6"/>
+      <c r="AW26" s="6"/>
+      <c r="AX26" s="6"/>
+      <c r="AY26" s="6"/>
+      <c r="AZ26" s="6"/>
+      <c r="BA26" s="6"/>
+      <c r="BB26" s="6"/>
+      <c r="BC26" s="6"/>
+      <c r="BD26" s="6"/>
+      <c r="BE26" s="6"/>
+      <c r="BF26" s="6"/>
+      <c r="BG26" s="6"/>
+      <c r="BH26" s="6"/>
+      <c r="BI26" s="6"/>
+      <c r="BJ26" s="6"/>
+      <c r="BK26" s="6"/>
+      <c r="BL26" s="6"/>
+      <c r="BM26" s="6"/>
+      <c r="BN26" s="6"/>
+      <c r="BO26" s="6"/>
+      <c r="BP26" s="6"/>
+      <c r="BQ26" s="6"/>
+      <c r="BR26" s="6"/>
+      <c r="BS26" s="6"/>
+      <c r="BT26" s="6"/>
+      <c r="BU26" s="6"/>
+      <c r="BV26" s="6"/>
+      <c r="BW26" s="6"/>
+      <c r="BX26" s="6"/>
+      <c r="BY26" s="6"/>
+      <c r="BZ26" s="6"/>
+      <c r="CA26" s="2"/>
+      <c r="CB26" s="2"/>
+      <c r="CC26" s="2"/>
+      <c r="CD26" s="2"/>
+      <c r="CE26" s="2"/>
+      <c r="CF26" s="2"/>
+      <c r="CG26" s="2"/>
+      <c r="CH26" s="2"/>
+      <c r="CI26" s="2"/>
+      <c r="CJ26" s="2"/>
+      <c r="CK26" s="2"/>
+      <c r="CL26" s="2"/>
+      <c r="CM26" s="2"/>
+      <c r="CN26" s="2"/>
+      <c r="CO26" s="6"/>
+    </row>
+    <row r="27" spans="1:101">
+      <c r="A27" s="10"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="6"/>
+      <c r="AG27" s="6"/>
+      <c r="AH27" s="6"/>
+      <c r="AI27" s="6"/>
+      <c r="AJ27" s="6"/>
+      <c r="AK27" s="6"/>
+      <c r="AL27" s="6"/>
+      <c r="AM27" s="6"/>
+      <c r="AN27" s="6"/>
+      <c r="AO27" s="6"/>
+      <c r="AP27" s="6"/>
+      <c r="AQ27" s="6"/>
+      <c r="AR27" s="6"/>
+      <c r="AS27" s="6"/>
+      <c r="AT27" s="6"/>
+      <c r="AU27" s="6"/>
+      <c r="AV27" s="6"/>
+      <c r="AW27" s="6"/>
+      <c r="AX27" s="6"/>
+      <c r="AY27" s="6"/>
+      <c r="AZ27" s="6"/>
+      <c r="BA27" s="6"/>
+      <c r="BB27" s="6"/>
+      <c r="BC27" s="6"/>
+      <c r="BD27" s="6"/>
+      <c r="BE27" s="6"/>
+      <c r="BF27" s="6"/>
+      <c r="BG27" s="6"/>
+      <c r="BH27" s="6"/>
+      <c r="BI27" s="6"/>
+      <c r="BJ27" s="6"/>
+      <c r="BK27" s="6"/>
+      <c r="BL27" s="6"/>
+      <c r="BM27" s="6"/>
+      <c r="BN27" s="6"/>
+      <c r="BO27" s="6"/>
+      <c r="BP27" s="6"/>
+      <c r="BQ27" s="6"/>
+      <c r="BR27" s="6"/>
+      <c r="BS27" s="6"/>
+      <c r="BT27" s="6"/>
+      <c r="BU27" s="6"/>
+      <c r="BV27" s="6"/>
+      <c r="BW27" s="6"/>
+      <c r="BX27" s="6"/>
+      <c r="BY27" s="6"/>
+      <c r="BZ27" s="6"/>
+      <c r="CA27" s="6"/>
+      <c r="CB27" s="6"/>
+      <c r="CC27" s="6"/>
+      <c r="CD27" s="6"/>
+      <c r="CE27" s="6"/>
+      <c r="CF27" s="6"/>
+      <c r="CG27" s="6"/>
+      <c r="CH27" s="6"/>
+    </row>
+    <row r="28" spans="1:101">
+      <c r="A28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="6"/>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="6"/>
+      <c r="AG28" s="6"/>
+      <c r="AH28" s="6"/>
+      <c r="AI28" s="6"/>
+      <c r="AJ28" s="6"/>
+      <c r="AK28" s="6"/>
+      <c r="AL28" s="6"/>
+      <c r="AM28" s="6"/>
+      <c r="AN28" s="6"/>
+      <c r="AO28" s="6"/>
+      <c r="AP28" s="6"/>
+      <c r="AQ28" s="6"/>
+      <c r="AR28" s="6"/>
+      <c r="AS28" s="6"/>
+      <c r="AT28" s="6"/>
+      <c r="AU28" s="6"/>
+      <c r="AV28" s="6"/>
+      <c r="AW28" s="6"/>
+      <c r="AX28" s="6"/>
+      <c r="AY28" s="6"/>
+      <c r="AZ28" s="6"/>
+      <c r="BA28" s="6"/>
+      <c r="BB28" s="6"/>
+      <c r="BC28" s="6"/>
+      <c r="BD28" s="6"/>
+      <c r="BE28" s="6"/>
+      <c r="BF28" s="6"/>
+      <c r="BG28" s="6"/>
+      <c r="BH28" s="6"/>
+      <c r="BI28" s="6"/>
+      <c r="BJ28" s="6"/>
+      <c r="BK28" s="6"/>
+      <c r="BL28" s="6"/>
+      <c r="BM28" s="6"/>
+      <c r="BN28" s="6"/>
+      <c r="BO28" s="6"/>
+      <c r="BP28" s="6"/>
+      <c r="BQ28" s="6"/>
+      <c r="BR28" s="6"/>
+      <c r="BS28" s="6"/>
+      <c r="BT28" s="6"/>
+      <c r="BU28" s="6"/>
+      <c r="BV28" s="6"/>
+      <c r="BW28" s="6"/>
+      <c r="BX28" s="6"/>
+      <c r="BY28" s="6"/>
+      <c r="BZ28" s="6"/>
+      <c r="CA28" s="6"/>
+      <c r="CB28" s="6"/>
+      <c r="CC28" s="6"/>
+      <c r="CD28" s="6"/>
+      <c r="CE28" s="6"/>
+      <c r="CF28" s="6"/>
+      <c r="CG28" s="6"/>
+      <c r="CH28" s="6"/>
+    </row>
+    <row r="29" spans="1:101">
+      <c r="A29" s="10"/>
+    </row>
+    <row r="30" spans="1:101">
+      <c r="A30" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+    </row>
+    <row r="31" spans="1:101">
+      <c r="A31" s="10"/>
+    </row>
+    <row r="32" spans="1:101">
+      <c r="A32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA32" s="6"/>
+      <c r="AD32" s="4"/>
+      <c r="AE32" s="4"/>
+      <c r="AF32" s="4"/>
+      <c r="AG32" s="4"/>
+      <c r="AH32" s="4"/>
+      <c r="AI32" s="4"/>
+      <c r="AJ32" s="4"/>
+      <c r="AK32" s="4"/>
+      <c r="AL32" s="4"/>
+      <c r="AM32" s="4"/>
+      <c r="AN32" s="4"/>
+      <c r="AO32" s="4"/>
+      <c r="AP32" s="4"/>
+      <c r="AQ32" s="4"/>
+      <c r="AR32" s="4"/>
+      <c r="AS32" s="4"/>
+      <c r="AT32" s="4"/>
+      <c r="AU32" s="4"/>
+      <c r="AV32" s="4"/>
+      <c r="AW32" s="4"/>
+      <c r="AX32" s="4"/>
+      <c r="AY32" s="4"/>
+      <c r="AZ32" s="4"/>
+      <c r="BA32" s="4"/>
+      <c r="BB32" s="4"/>
+      <c r="BC32" s="4"/>
+      <c r="BD32" s="4"/>
+      <c r="BE32" s="4"/>
+      <c r="BF32" s="4"/>
+      <c r="BG32" s="4"/>
+      <c r="BH32" s="4"/>
+      <c r="BI32" s="4"/>
+      <c r="BJ32" s="4"/>
+      <c r="BK32" s="4"/>
+      <c r="BL32" s="4"/>
+      <c r="BM32" s="4"/>
+      <c r="BN32" s="4"/>
+      <c r="BO32" s="4"/>
+      <c r="BP32" s="4"/>
+      <c r="BQ32" s="4"/>
+      <c r="BR32" s="4"/>
+      <c r="BS32" s="4"/>
+      <c r="BT32" s="4"/>
+    </row>
+    <row r="33" spans="1:101">
+      <c r="A33" s="10"/>
+      <c r="AH33" s="6"/>
+    </row>
+    <row r="34" spans="1:101">
+      <c r="A34" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="CA34" s="2"/>
+      <c r="CB34" s="2"/>
+      <c r="CC34" s="2"/>
+      <c r="CD34" s="2"/>
+      <c r="CE34" s="2"/>
+      <c r="CF34" s="2"/>
+      <c r="CG34" s="2"/>
+    </row>
+    <row r="35" spans="1:101">
+      <c r="A35" s="10"/>
+    </row>
+    <row r="36" spans="1:101">
+      <c r="A36" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="2"/>
+      <c r="AG36" s="2"/>
+      <c r="AH36" s="2"/>
+      <c r="AI36" s="2"/>
+      <c r="AJ36" s="2"/>
+      <c r="AK36" s="2"/>
+      <c r="AL36" s="2"/>
+      <c r="AM36" s="2"/>
+      <c r="AN36" s="2"/>
+      <c r="AO36" s="2"/>
+      <c r="AP36" s="2"/>
+      <c r="AQ36" s="2"/>
+      <c r="AR36" s="2"/>
+      <c r="AS36" s="2"/>
+      <c r="AT36" s="2"/>
+      <c r="AU36" s="2"/>
+      <c r="AV36" s="2"/>
+      <c r="AW36" s="2"/>
+      <c r="AX36" s="2"/>
+      <c r="AY36" s="2"/>
+      <c r="AZ36" s="2"/>
+      <c r="BA36" s="2"/>
+      <c r="BB36" s="2"/>
+      <c r="BC36" s="2"/>
+      <c r="BD36" s="2"/>
+      <c r="BE36" s="2"/>
+      <c r="BF36" s="2"/>
+      <c r="BG36" s="2"/>
+      <c r="BH36" s="2"/>
+      <c r="BI36" s="2"/>
+      <c r="BJ36" s="2"/>
+      <c r="BK36" s="2"/>
+      <c r="BL36" s="2"/>
+      <c r="BM36" s="2"/>
+      <c r="BN36" s="2"/>
+      <c r="BO36" s="2"/>
+      <c r="BP36" s="2"/>
+      <c r="BQ36" s="2"/>
+      <c r="BR36" s="2"/>
+      <c r="BS36" s="2"/>
+      <c r="BT36" s="2"/>
+      <c r="BU36" s="2"/>
+      <c r="BV36" s="2"/>
+      <c r="BW36" s="2"/>
+      <c r="BX36" s="2"/>
+      <c r="BY36" s="2"/>
+      <c r="BZ36" s="2"/>
+      <c r="CA36" s="2"/>
+      <c r="CB36" s="2"/>
+      <c r="CC36" s="2"/>
+      <c r="CD36" s="2"/>
+      <c r="CE36" s="2"/>
+      <c r="CF36" s="2"/>
+      <c r="CG36" s="2"/>
+      <c r="CH36" s="2"/>
+      <c r="CI36" s="2"/>
+      <c r="CJ36" s="2"/>
+      <c r="CK36" s="2"/>
+      <c r="CL36" s="2"/>
+      <c r="CM36" s="2"/>
+      <c r="CN36" s="2"/>
+      <c r="CO36" s="2"/>
+      <c r="CP36" s="2"/>
+      <c r="CQ36" s="2"/>
+      <c r="CR36" s="2"/>
+      <c r="CS36" s="2"/>
+      <c r="CT36" s="2"/>
+      <c r="CU36" s="2"/>
+      <c r="CV36" s="2"/>
+      <c r="CW36" s="7"/>
+    </row>
+    <row r="37" spans="1:101">
+      <c r="A37" s="10"/>
+      <c r="AM37" s="6"/>
+    </row>
+    <row r="38" spans="1:101">
+      <c r="A38" s="10"/>
+    </row>
+    <row r="39" spans="1:101">
+      <c r="A39" s="10"/>
+    </row>
+    <row r="40" spans="1:101">
+      <c r="A40" s="10"/>
+    </row>
+    <row r="41" spans="1:101">
+      <c r="A41" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="AG1:AM1"/>
+    <mergeCell ref="CD1:CJ1"/>
+    <mergeCell ref="CK1:CQ1"/>
     <mergeCell ref="CR1:CV1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="N2:AR2"/>
@@ -1941,9 +3241,6 @@
     <mergeCell ref="L1:R1"/>
     <mergeCell ref="S1:Y1"/>
     <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
-    <mergeCell ref="CD1:CJ1"/>
-    <mergeCell ref="CK1:CQ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Vergaderverslagen klaar + taakstructuur aangepast
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab56a76f82895e8b/Documents/2022-2023 KULAK B1/2022-2023 Probleemoplossen en ontwerpen 2/2022_2023_Probleemoplossen_en_Ontwerpen_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emile\OneDrive\Documenten\P&amp;O 2\GIT\2022_2023_Probleemoplossen_en_Ontwerpen_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E611CA62-36F7-4A12-B88E-10AB52355B0D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234CCC50-6233-4D81-A1D2-96A4A2A5FF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -237,7 +237,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -554,8 +554,8 @@
   </sheetPr>
   <dimension ref="A1:CX41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CE87" sqref="CE87"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1984,11 +1984,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
-    <mergeCell ref="CD1:CJ1"/>
     <mergeCell ref="CK1:CQ1"/>
     <mergeCell ref="CR1:CV1"/>
     <mergeCell ref="B2:M2"/>
@@ -2003,6 +1998,11 @@
     <mergeCell ref="BW1:CC1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
+    <mergeCell ref="CD1:CJ1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="28" orientation="landscape" r:id="rId1"/>

</xml_diff>